<commit_message>
log files, updated report
</commit_message>
<xml_diff>
--- a/CITS3402AssignmentData2.xlsx
+++ b/CITS3402AssignmentData2.xlsx
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>ArraySIzeLog2</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>LogTimeToCompute</t>
-  </si>
-  <si>
-    <t>Scalar Multiplication</t>
   </si>
   <si>
     <t>ArraySize</t>
@@ -61,9 +58,6 @@
   </si>
   <si>
     <t>logTimeToCompute 1</t>
-  </si>
-  <si>
-    <t>16 THREADS 1</t>
   </si>
   <si>
     <t>AVG</t>
@@ -97,6 +91,21 @@
   </si>
   <si>
     <t>RUNNING ALGORITHM 1</t>
+  </si>
+  <si>
+    <t>NUMBER OF PROCESSES</t>
+  </si>
+  <si>
+    <t>NUMBER OF NODES</t>
+  </si>
+  <si>
+    <t>512 Vertices.     1</t>
+  </si>
+  <si>
+    <t>2048 Vertices.       1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1246,11 +1255,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2036526528"/>
-        <c:axId val="2036528656"/>
+        <c:axId val="-773212192"/>
+        <c:axId val="-773231056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2036526528"/>
+        <c:axId val="-773212192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1356,12 +1365,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2036528656"/>
+        <c:crossAx val="-773231056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2036528656"/>
+        <c:axId val="-773231056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1470,7 +1479,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2036526528"/>
+        <c:crossAx val="-773212192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1617,7 +1626,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1641,7 +1650,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$88:$G$88</c:f>
+              <c:f>Sheet1!$C$90:$G$90</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1725,31 +1734,19 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$39:$G$39</c:f>
+              <c:f>Sheet1!$C$41:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024.0</c:v>
+                  <c:v>205.43103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$95:$G$95</c:f>
+              <c:f>Sheet1!$C$97:$G$97</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1766,11 +1763,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2115214304"/>
-        <c:axId val="2115217424"/>
+        <c:axId val="-747437744"/>
+        <c:axId val="-753504608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2115214304"/>
+        <c:axId val="-747437744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1820,7 +1817,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1882,12 +1878,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115217424"/>
+        <c:crossAx val="-753504608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2115217424"/>
+        <c:axId val="-753504608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1932,7 +1928,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1995,7 +1990,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115214304"/>
+        <c:crossAx val="-747437744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2009,7 +2004,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2181,7 +2175,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2205,7 +2199,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$104:$G$104</c:f>
+              <c:f>Sheet1!$C$106:$G$106</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2289,31 +2283,19 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$39:$G$39</c:f>
+              <c:f>Sheet1!$C$41:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024.0</c:v>
+                  <c:v>205.43103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$108:$G$108</c:f>
+              <c:f>Sheet1!$C$110:$G$110</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2390,31 +2372,19 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$39:$G$39</c:f>
+              <c:f>Sheet1!$C$41:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024.0</c:v>
+                  <c:v>205.43103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$112:$G$112</c:f>
+              <c:f>Sheet1!$C$114:$G$114</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2431,11 +2401,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2115245776"/>
-        <c:axId val="2115248896"/>
+        <c:axId val="-747330480"/>
+        <c:axId val="-747327024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2115245776"/>
+        <c:axId val="-747330480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2485,7 +2455,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2514,6 +2483,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2547,12 +2517,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115248896"/>
+        <c:crossAx val="-747327024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2115248896"/>
+        <c:axId val="-747327024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2597,7 +2567,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2660,7 +2629,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115245776"/>
+        <c:crossAx val="-747330480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2674,7 +2643,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2964,10 +2932,25 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$26:$G$26</c:f>
+              <c:f>Sheet1!$C$27:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3065,10 +3048,25 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$37:$G$37</c:f>
+              <c:f>Sheet1!$C$39:$G$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3082,11 +3080,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2037213168"/>
-        <c:axId val="2036581872"/>
+        <c:axId val="-773079280"/>
+        <c:axId val="-773191696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2037213168"/>
+        <c:axId val="-773079280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5.0"/>
@@ -3194,12 +3192,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2036581872"/>
+        <c:crossAx val="-773191696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2036581872"/>
+        <c:axId val="-773191696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3306,7 +3304,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2037213168"/>
+        <c:crossAx val="-773079280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3474,34 +3472,25 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$39:$G$39</c:f>
+              <c:f>Sheet1!$C$41:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024.0</c:v>
+                  <c:v>205.43103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$40:$G$40</c:f>
+              <c:f>Sheet1!$C$42:$G$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>198.982697</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3548,31 +3537,19 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$39:$G$39</c:f>
+              <c:f>Sheet1!$C$41:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024.0</c:v>
+                  <c:v>205.43103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$41:$G$41</c:f>
+              <c:f>Sheet1!$C$43:$G$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3622,31 +3599,19 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$39:$G$39</c:f>
+              <c:f>Sheet1!$C$41:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024.0</c:v>
+                  <c:v>205.43103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$42:$G$42</c:f>
+              <c:f>Sheet1!$C$44:$G$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3696,31 +3661,19 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$39:$G$39</c:f>
+              <c:f>Sheet1!$C$41:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024.0</c:v>
+                  <c:v>205.43103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$43:$G$43</c:f>
+              <c:f>Sheet1!$C$45:$G$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3770,31 +3723,19 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$39:$G$39</c:f>
+              <c:f>Sheet1!$C$41:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024.0</c:v>
+                  <c:v>205.43103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$44:$G$44</c:f>
+              <c:f>Sheet1!$C$46:$G$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3811,11 +3752,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2115025408"/>
-        <c:axId val="2115015760"/>
+        <c:axId val="-774057744"/>
+        <c:axId val="-774047936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2115025408"/>
+        <c:axId val="-774057744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3920,12 +3861,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115015760"/>
+        <c:crossAx val="-774047936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2115015760"/>
+        <c:axId val="-774047936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4034,7 +3975,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115025408"/>
+        <c:crossAx val="-774057744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4181,31 +4122,19 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$39:$G$39</c:f>
+              <c:f>Sheet1!$C$41:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024.0</c:v>
+                  <c:v>205.43103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$45:$G$45</c:f>
+              <c:f>Sheet1!$C$47:$G$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4289,31 +4218,19 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$39:$G$39</c:f>
+              <c:f>Sheet1!$C$41:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024.0</c:v>
+                  <c:v>205.43103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$51:$G$51</c:f>
+              <c:f>Sheet1!$C$53:$G$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4397,31 +4314,19 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$39:$G$39</c:f>
+              <c:f>Sheet1!$C$41:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024.0</c:v>
+                  <c:v>205.43103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$57:$G$57</c:f>
+              <c:f>Sheet1!$C$59:$G$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4438,11 +4343,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2115036144"/>
-        <c:axId val="2115038848"/>
+        <c:axId val="-773904704"/>
+        <c:axId val="-773901584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2115036144"/>
+        <c:axId val="-773904704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4554,12 +4459,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115038848"/>
+        <c:crossAx val="-773901584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2115038848"/>
+        <c:axId val="-773901584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4667,7 +4572,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115036144"/>
+        <c:crossAx val="-773904704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4821,7 +4726,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4845,7 +4750,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$62:$G$62</c:f>
+              <c:f>Sheet1!$C$64:$G$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4898,7 +4803,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4922,7 +4827,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$63:$G$63</c:f>
+              <c:f>Sheet1!$C$65:$G$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4975,7 +4880,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4999,7 +4904,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$64:$G$64</c:f>
+              <c:f>Sheet1!$C$66:$G$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5052,7 +4957,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5076,7 +4981,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$65:$G$65</c:f>
+              <c:f>Sheet1!$C$67:$G$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5129,7 +5034,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5153,7 +5058,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$66:$G$66</c:f>
+              <c:f>Sheet1!$C$68:$G$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5219,7 +5124,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5243,7 +5148,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$62:$G$62</c:f>
+              <c:f>Sheet1!$C$64:$G$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5293,7 +5198,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5317,7 +5222,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$63:$G$63</c:f>
+              <c:f>Sheet1!$C$65:$G$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5367,7 +5272,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5391,7 +5296,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$64:$G$64</c:f>
+              <c:f>Sheet1!$C$66:$G$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5441,7 +5346,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5465,7 +5370,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$65:$G$65</c:f>
+              <c:f>Sheet1!$C$67:$G$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5515,7 +5420,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5539,7 +5444,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$66:$G$66</c:f>
+              <c:f>Sheet1!$C$68:$G$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5556,11 +5461,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2115095072"/>
-        <c:axId val="2115098192"/>
+        <c:axId val="-773959264"/>
+        <c:axId val="-773956144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2115095072"/>
+        <c:axId val="-773959264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5606,7 +5511,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5666,12 +5570,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115098192"/>
+        <c:crossAx val="-773956144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2115098192"/>
+        <c:axId val="-773956144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5717,7 +5621,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5780,7 +5683,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115095072"/>
+        <c:crossAx val="-773959264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5920,7 +5823,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5944,7 +5847,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$67:$G$67</c:f>
+              <c:f>Sheet1!$C$69:$G$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -6028,7 +5931,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -6052,7 +5955,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$73:$G$73</c:f>
+              <c:f>Sheet1!$C$75:$G$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -6136,31 +6039,19 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$39:$G$39</c:f>
+              <c:f>Sheet1!$C$41:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024.0</c:v>
+                  <c:v>205.43103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$79:$G$79</c:f>
+              <c:f>Sheet1!$C$81:$G$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -6177,11 +6068,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2115127872"/>
-        <c:axId val="2115130992"/>
+        <c:axId val="-773928912"/>
+        <c:axId val="-773925792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2115127872"/>
+        <c:axId val="-773928912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6231,7 +6122,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6294,12 +6184,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115130992"/>
+        <c:crossAx val="-773925792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2115130992"/>
+        <c:axId val="-773925792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6344,7 +6234,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6407,7 +6296,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115127872"/>
+        <c:crossAx val="-773928912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6421,7 +6310,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6983,11 +6871,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2115156688"/>
-        <c:axId val="2115159808"/>
+        <c:axId val="-750556400"/>
+        <c:axId val="-750553280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2115156688"/>
+        <c:axId val="-750556400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5.0"/>
@@ -7094,12 +6982,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115159808"/>
+        <c:crossAx val="-750553280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2115159808"/>
+        <c:axId val="-750553280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7208,7 +7096,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115156688"/>
+        <c:crossAx val="-750556400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7337,7 +7225,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -7361,7 +7249,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$83:$G$83</c:f>
+              <c:f>Sheet1!$C$85:$G$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -7411,7 +7299,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -7435,7 +7323,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$84:$G$84</c:f>
+              <c:f>Sheet1!$C$86:$G$86</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -7485,7 +7373,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -7509,7 +7397,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$85:$G$85</c:f>
+              <c:f>Sheet1!$C$87:$G$87</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -7559,7 +7447,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -7583,7 +7471,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$86:$G$86</c:f>
+              <c:f>Sheet1!$C$88:$G$88</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -7633,7 +7521,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -7657,7 +7545,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$87:$G$87</c:f>
+              <c:f>Sheet1!$C$89:$G$89</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -7674,11 +7562,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2115196224"/>
-        <c:axId val="2115199344"/>
+        <c:axId val="-874553632"/>
+        <c:axId val="-874550512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2115196224"/>
+        <c:axId val="-874553632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7724,7 +7612,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7783,12 +7670,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115199344"/>
+        <c:crossAx val="-874550512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2115199344"/>
+        <c:axId val="-874550512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7834,7 +7721,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7897,7 +7783,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115196224"/>
+        <c:crossAx val="-874553632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8026,7 +7912,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -8050,7 +7936,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$99:$G$99</c:f>
+              <c:f>Sheet1!$C$101:$G$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -8100,7 +7986,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -8124,7 +8010,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$100:$G$100</c:f>
+              <c:f>Sheet1!$C$102:$G$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -8174,7 +8060,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -8198,7 +8084,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$101:$G$101</c:f>
+              <c:f>Sheet1!$C$103:$G$103</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -8248,7 +8134,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -8272,7 +8158,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$102:$G$102</c:f>
+              <c:f>Sheet1!$C$104:$G$104</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -8322,7 +8208,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$G$61</c:f>
+              <c:f>Sheet1!$C$63:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -8346,7 +8232,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$103:$G$103</c:f>
+              <c:f>Sheet1!$C$105:$G$105</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -8363,11 +8249,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2084733216"/>
-        <c:axId val="2084735440"/>
+        <c:axId val="-747616384"/>
+        <c:axId val="-747613680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2084733216"/>
+        <c:axId val="-747616384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8413,7 +8299,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8472,12 +8357,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2084735440"/>
+        <c:crossAx val="-747613680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2084735440"/>
+        <c:axId val="-747613680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8523,7 +8408,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8586,7 +8470,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2084733216"/>
+        <c:crossAx val="-747616384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14846,7 +14730,7 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>212722</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>130561</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -14870,13 +14754,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>232362</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>141261</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>652438</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>189907</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -14900,13 +14784,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>90508</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>165945</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>517234</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>39372</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -14930,13 +14814,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>201814</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>9235</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>659014</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>115454</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -14960,13 +14844,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>126076</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>16625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>552802</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>97871</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -14998,7 +14882,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>823603</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>71215</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -15024,13 +14908,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>229518</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>686718</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>97</xdr:row>
       <xdr:rowOff>106218</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -15056,13 +14940,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>260120</xdr:colOff>
-      <xdr:row>97</xdr:row>
+      <xdr:row>99</xdr:row>
       <xdr:rowOff>107108</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>717320</xdr:colOff>
-      <xdr:row>111</xdr:row>
+      <xdr:row>113</xdr:row>
       <xdr:rowOff>14411</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -15088,13 +14972,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>268111</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>42334</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>296333</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>97</xdr:row>
       <xdr:rowOff>165914</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -15120,13 +15004,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>386080</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>193040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>139982</xdr:colOff>
-      <xdr:row>112</xdr:row>
+      <xdr:row>114</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -15154,7 +15038,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="43730.69662476852" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="5">
   <cacheSource type="worksheet">
-    <worksheetSource ref="C39:G44" sheet="Sheet1"/>
+    <worksheetSource ref="C41:G46" sheet="Sheet1"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="64" numFmtId="0">
@@ -15222,7 +15106,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C20" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
@@ -15608,10 +15492,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H112"/>
+  <dimension ref="B1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" zoomScaleNormal="142" zoomScalePageLayoutView="142" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="125" zoomScaleNormal="142" zoomScalePageLayoutView="142" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15621,7 +15505,7 @@
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B1" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
@@ -15651,7 +15535,7 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>32</v>
@@ -15771,7 +15655,7 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -15906,7 +15790,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
@@ -15916,7 +15800,7 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1">
         <v>4.7699999999999999E-4</v>
@@ -16016,7 +15900,7 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21">
         <f>LOG(C16,2)</f>
@@ -16139,148 +16023,196 @@
         <v>9.0453009452010136</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-    </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="G27" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="C27" s="12">
+        <v>1</v>
+      </c>
+      <c r="D27" s="12">
+        <v>2</v>
+      </c>
+      <c r="E27" s="12">
+        <v>4</v>
+      </c>
+      <c r="F27" s="12">
+        <v>8</v>
+      </c>
+      <c r="G27" s="12">
+        <v>16</v>
+      </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="13">
-        <v>2</v>
-      </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+      <c r="B28" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="12">
+        <f>C27*12</f>
+        <v>12</v>
+      </c>
+      <c r="D28" s="12">
+        <f t="shared" ref="D28:G28" si="5">D27*12</f>
+        <v>24</v>
+      </c>
+      <c r="E28" s="12">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+      <c r="F28" s="12">
+        <f t="shared" si="5"/>
+        <v>96</v>
+      </c>
+      <c r="G28" s="12">
+        <f t="shared" si="5"/>
+        <v>192</v>
+      </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="13">
-        <v>3</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="B29" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1.759835</v>
+      </c>
+      <c r="D29">
+        <v>8.3139470000000006</v>
+      </c>
+      <c r="E29">
+        <v>9.6073350000000008</v>
+      </c>
+      <c r="F29">
+        <v>12.640995</v>
+      </c>
+      <c r="G29" s="1">
+        <v>14.531649</v>
+      </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B30" s="13">
-        <v>4</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C30" s="1"/>
       <c r="D30" s="1"/>
+      <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B31" s="13">
-        <v>5</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="F31" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="13" t="s">
-        <v>9</v>
-      </c>
+      <c r="B32" s="13">
+        <v>4</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" s="13">
+        <v>5</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B34" s="13">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B36" s="13">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B35" s="13">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B37" s="13">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B36" s="13">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B38" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B39" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="12">
+        <v>1</v>
+      </c>
+      <c r="D39" s="12">
+        <v>2</v>
+      </c>
+      <c r="E39" s="12">
+        <v>4</v>
+      </c>
+      <c r="F39" s="12">
         <v>8</v>
       </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
+      <c r="G39" s="12">
+        <v>16</v>
+      </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="11" t="s">
-        <v>3</v>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B40" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="12">
+        <f>C39*12</f>
+        <v>12</v>
+      </c>
+      <c r="D40" s="12">
+        <f t="shared" ref="D40" si="6">D39*12</f>
+        <v>24</v>
+      </c>
+      <c r="E40" s="12">
+        <f t="shared" ref="E40" si="7">E39*12</f>
+        <v>48</v>
+      </c>
+      <c r="F40" s="12">
+        <f t="shared" ref="F40" si="8">F39*12</f>
+        <v>96</v>
+      </c>
+      <c r="G40" s="12">
+        <f t="shared" ref="G40" si="9">G39*12</f>
+        <v>192</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39">
-        <v>64</v>
-      </c>
-      <c r="D39">
-        <v>128</v>
-      </c>
-      <c r="E39">
-        <v>256</v>
-      </c>
-      <c r="F39">
-        <v>512</v>
-      </c>
-      <c r="G39">
-        <v>1024</v>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B41" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41">
+        <v>205.43102999999999</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B41">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B42">
         <v>2</v>
       </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B42">
-        <v>3</v>
-      </c>
-      <c r="C42" s="1"/>
+      <c r="C42">
+        <v>198.982697</v>
+      </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B43">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -16288,9 +16220,9 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B44">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -16298,19 +16230,19 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B46">
-        <v>1</v>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>24</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -16318,41 +16250,39 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B47">
-        <v>2</v>
-      </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B48">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B49">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B50">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -16362,19 +16292,19 @@
       <c r="H50" s="1"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
       <c r="H51" s="1"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B52">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -16384,19 +16314,19 @@
       <c r="H52" s="1"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B53">
-        <v>2</v>
-      </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
       <c r="H53" s="1"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B54">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -16407,7 +16337,7 @@
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B55">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -16418,7 +16348,7 @@
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B56">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -16428,71 +16358,73 @@
       <c r="H56" s="1"/>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
-        <v>8</v>
-      </c>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
       <c r="H57" s="1"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B58">
+        <v>5</v>
+      </c>
+      <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
     </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="1"/>
+    </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B60" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
-        <v>4</v>
-      </c>
-      <c r="C61" s="11">
-        <v>64</v>
-      </c>
-      <c r="D61" s="11">
-        <v>128</v>
-      </c>
-      <c r="E61" s="11">
-        <v>256</v>
-      </c>
-      <c r="F61" s="11">
-        <v>512</v>
-      </c>
-      <c r="G61" s="11">
-        <v>1024</v>
-      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B62" t="s">
-        <v>1</v>
-      </c>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
+      <c r="B62" s="11" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B63">
-        <v>2</v>
-      </c>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
+      <c r="B63" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" s="11">
+        <v>64</v>
+      </c>
+      <c r="D63" s="11">
+        <v>128</v>
+      </c>
+      <c r="E63" s="11">
+        <v>256</v>
+      </c>
+      <c r="F63" s="11">
+        <v>512</v>
+      </c>
+      <c r="G63" s="11">
+        <v>1024</v>
+      </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B64">
-        <v>3</v>
+      <c r="B64" t="s">
+        <v>1</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -16502,7 +16434,7 @@
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B65">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -16512,7 +16444,7 @@
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B66">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -16521,18 +16453,18 @@
       <c r="G66" s="1"/>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
-        <v>11</v>
-      </c>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
+      <c r="B67">
+        <v>4</v>
+      </c>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
-        <v>12</v>
+      <c r="B68">
+        <v>5</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -16541,18 +16473,18 @@
       <c r="G68" s="1"/>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B69">
-        <v>2</v>
-      </c>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
+      <c r="B69" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B70">
-        <v>3</v>
+      <c r="B70" t="s">
+        <v>10</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -16562,7 +16494,7 @@
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B71">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -16572,7 +16504,7 @@
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B72">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -16581,15 +16513,18 @@
       <c r="G72" s="1"/>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C73" s="12"/>
-      <c r="D73" s="12"/>
-      <c r="E73" s="12"/>
-      <c r="F73" s="12"/>
-      <c r="G73" s="12"/>
+      <c r="B73">
+        <v>4</v>
+      </c>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B74" t="s">
-        <v>13</v>
+      <c r="B74">
+        <v>5</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -16598,18 +16533,15 @@
       <c r="G74" s="1"/>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B75">
-        <v>2</v>
-      </c>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B76">
-        <v>3</v>
+      <c r="B76" t="s">
+        <v>11</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -16619,7 +16551,7 @@
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B77">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -16629,7 +16561,7 @@
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B78">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -16638,60 +16570,60 @@
       <c r="G78" s="1"/>
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C79" s="12"/>
-      <c r="D79" s="12"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
-      <c r="G79" s="12"/>
+      <c r="B79">
+        <v>4</v>
+      </c>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B80">
+        <v>5</v>
+      </c>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B81" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C81" s="11">
-        <v>64</v>
-      </c>
-      <c r="D81" s="11">
-        <v>128</v>
-      </c>
-      <c r="E81" s="11">
-        <v>256</v>
-      </c>
-      <c r="F81" s="11">
-        <v>512</v>
-      </c>
-      <c r="G81" s="11">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B82" t="s">
-        <v>15</v>
-      </c>
+      <c r="C81" s="12"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="12"/>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B83">
-        <v>1</v>
-      </c>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
+      <c r="B83" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C83" s="11">
+        <v>64</v>
+      </c>
+      <c r="D83" s="11">
+        <v>128</v>
+      </c>
+      <c r="E83" s="11">
+        <v>256</v>
+      </c>
+      <c r="F83" s="11">
+        <v>512</v>
+      </c>
+      <c r="G83" s="11">
+        <v>1024</v>
+      </c>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B84">
-        <v>2</v>
-      </c>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
+      <c r="B84" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B85">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -16701,7 +16633,7 @@
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B86">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
@@ -16711,7 +16643,7 @@
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B87">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -16720,45 +16652,45 @@
       <c r="G87" s="1"/>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C88" s="14"/>
-      <c r="D88" s="14"/>
-      <c r="E88" s="14"/>
-      <c r="F88" s="14"/>
-      <c r="G88" s="14"/>
+      <c r="B88">
+        <v>4</v>
+      </c>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B89" t="s">
-        <v>16</v>
-      </c>
-      <c r="C89" s="12"/>
-      <c r="D89" s="12"/>
-      <c r="E89" s="12"/>
-      <c r="F89" s="12"/>
-      <c r="G89" s="12"/>
+      <c r="B89">
+        <v>5</v>
+      </c>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B90">
-        <v>1</v>
-      </c>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="1"/>
-      <c r="F90" s="1"/>
-      <c r="G90" s="1"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B91">
-        <v>2</v>
-      </c>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
-      <c r="E91" s="1"/>
-      <c r="F91" s="1"/>
-      <c r="G91" s="1"/>
+      <c r="B91" t="s">
+        <v>14</v>
+      </c>
+      <c r="C91" s="12"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="12"/>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B92">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
@@ -16768,7 +16700,7 @@
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B93">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
@@ -16778,7 +16710,7 @@
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B94">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
@@ -16787,68 +16719,68 @@
       <c r="G94" s="1"/>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C95" s="14"/>
-      <c r="D95" s="14"/>
-      <c r="E95" s="14"/>
-      <c r="F95" s="14"/>
-      <c r="G95" s="14"/>
+      <c r="B95">
+        <v>4</v>
+      </c>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
     </row>
     <row r="96" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C96" s="12"/>
-      <c r="D96" s="12"/>
-      <c r="E96" s="12"/>
-      <c r="F96" s="12"/>
-      <c r="G96" s="12"/>
+      <c r="B96">
+        <v>5</v>
+      </c>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B97" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C97" s="11">
-        <v>64</v>
-      </c>
-      <c r="D97" s="11">
-        <v>128</v>
-      </c>
-      <c r="E97" s="11">
-        <v>256</v>
-      </c>
-      <c r="F97" s="11">
-        <v>512</v>
-      </c>
-      <c r="G97" s="11">
-        <v>1024</v>
-      </c>
+      <c r="C97" s="14"/>
+      <c r="D97" s="14"/>
+      <c r="E97" s="14"/>
+      <c r="F97" s="14"/>
+      <c r="G97" s="14"/>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B98" t="s">
-        <v>15</v>
-      </c>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="12"/>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B99">
-        <v>1</v>
-      </c>
-      <c r="D99" s="1"/>
-      <c r="E99" s="1"/>
-      <c r="F99" s="1"/>
-      <c r="G99" s="1"/>
+      <c r="B99" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" s="11">
+        <v>64</v>
+      </c>
+      <c r="D99" s="11">
+        <v>128</v>
+      </c>
+      <c r="E99" s="11">
+        <v>256</v>
+      </c>
+      <c r="F99" s="11">
+        <v>512</v>
+      </c>
+      <c r="G99" s="11">
+        <v>1024</v>
+      </c>
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B100">
-        <v>2</v>
-      </c>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
-      <c r="F100" s="1"/>
-      <c r="G100" s="1"/>
+      <c r="B100" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B101">
-        <v>3</v>
-      </c>
-      <c r="C101" s="1"/>
+        <v>1</v>
+      </c>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
@@ -16856,7 +16788,7 @@
     </row>
     <row r="102" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B102">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
@@ -16866,7 +16798,7 @@
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B103">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
@@ -16875,15 +16807,18 @@
       <c r="G103" s="1"/>
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C104" s="12"/>
-      <c r="D104" s="12"/>
-      <c r="E104" s="12"/>
-      <c r="F104" s="12"/>
-      <c r="G104" s="12"/>
+      <c r="B104">
+        <v>4</v>
+      </c>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B105" s="13" t="s">
-        <v>18</v>
+      <c r="B105">
+        <v>5</v>
       </c>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
@@ -16892,18 +16827,15 @@
       <c r="G105" s="1"/>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B106">
-        <v>2</v>
-      </c>
-      <c r="C106" s="1"/>
-      <c r="D106" s="1"/>
-      <c r="E106" s="1"/>
-      <c r="F106" s="1"/>
-      <c r="G106" s="1"/>
+      <c r="C106" s="12"/>
+      <c r="D106" s="12"/>
+      <c r="E106" s="12"/>
+      <c r="F106" s="12"/>
+      <c r="G106" s="12"/>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B107">
-        <v>3</v>
+      <c r="B107" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
@@ -16912,16 +16844,19 @@
       <c r="G107" s="1"/>
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B108" t="s">
-        <v>19</v>
-      </c>
-      <c r="C108" s="12"/>
-      <c r="D108" s="12"/>
-      <c r="E108" s="12"/>
-      <c r="F108" s="12"/>
-      <c r="G108" s="12"/>
+      <c r="B108">
+        <v>2</v>
+      </c>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
     </row>
     <row r="109" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B109">
+        <v>3</v>
+      </c>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
@@ -16929,11 +16864,14 @@
       <c r="G109" s="1"/>
     </row>
     <row r="110" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C110" s="1"/>
-      <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
-      <c r="F110" s="1"/>
-      <c r="G110" s="1"/>
+      <c r="B110" t="s">
+        <v>17</v>
+      </c>
+      <c r="C110" s="12"/>
+      <c r="D110" s="12"/>
+      <c r="E110" s="12"/>
+      <c r="F110" s="12"/>
+      <c r="G110" s="12"/>
     </row>
     <row r="111" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C111" s="1"/>
@@ -16943,11 +16881,25 @@
       <c r="G111" s="1"/>
     </row>
     <row r="112" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C112" s="12"/>
-      <c r="D112" s="12"/>
-      <c r="E112" s="12"/>
-      <c r="F112" s="12"/>
-      <c r="G112" s="12"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="1"/>
+      <c r="G112" s="1"/>
+    </row>
+    <row r="113" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
+      <c r="G113" s="1"/>
+    </row>
+    <row r="114" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C114" s="12"/>
+      <c r="D114" s="12"/>
+      <c r="E114" s="12"/>
+      <c r="F114" s="12"/>
+      <c r="G114" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>